<commit_message>
adding feature files and step definitions
</commit_message>
<xml_diff>
--- a/src/test/resources/users.xlsx
+++ b/src/test/resources/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -106,6 +106,23 @@
   </si>
   <si>
     <t>Mobile number</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>a@z3.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
   <si>
     <t>Mr.</t>
@@ -214,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -232,6 +249,93 @@
       <top style="thin">
         <color indexed="10"/>
       </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -334,13 +438,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -350,28 +485,64 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1465,14 +1636,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="8.85156" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="5" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1485,6 +1656,8 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
@@ -1496,6 +1669,64 @@
       <c r="C2" t="s" s="2">
         <v>5</v>
       </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1514,58 +1745,107 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="3" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="12" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.55" customHeight="1">
-      <c r="A1" t="s" s="4">
+      <c r="A1" t="s" s="13">
         <v>6</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" ht="13.1" customHeight="1">
-      <c r="A2" t="s" s="7">
+      <c r="A2" t="s" s="16">
         <v>0</v>
       </c>
-      <c r="B2" t="s" s="7">
+      <c r="B2" t="s" s="16">
         <v>7</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="C2" t="s" s="16">
         <v>8</v>
       </c>
-      <c r="D2" t="s" s="7">
+      <c r="D2" t="s" s="16">
         <v>9</v>
       </c>
-      <c r="E2" t="s" s="7">
+      <c r="E2" t="s" s="16">
         <v>10</v>
       </c>
     </row>
     <row r="3" ht="13.1" customHeight="1">
-      <c r="A3" t="s" s="8">
+      <c r="A3" t="s" s="17">
         <v>3</v>
       </c>
-      <c r="B3" t="s" s="9">
+      <c r="B3" t="s" s="18">
         <v>11</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="19">
         <v>123</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="19">
         <v>3</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="19">
         <v>2025</v>
       </c>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1581,14 +1861,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="8.85156" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="8.85156" style="11" customWidth="1"/>
+    <col min="1" max="5" width="8.85156" style="23" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1601,6 +1881,8 @@
       <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
@@ -1612,6 +1894,64 @@
       <c r="C2" t="s" s="2">
         <v>14</v>
       </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1624,14 +1964,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="16" width="8.85156" style="12" customWidth="1"/>
-    <col min="17" max="16384" width="8.85156" style="12" customWidth="1"/>
+    <col min="1" max="16" width="8.85156" style="24" customWidth="1"/>
+    <col min="17" max="16384" width="8.85156" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1686,57 +2026,201 @@
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M2" t="s" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="N2" t="s" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="O2" t="s" s="2">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P2" t="s" s="2">
-        <v>40</v>
-      </c>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="10"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="10"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="10"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="10"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="" tooltip="" display="aditya@p.com"/>
+    <hyperlink ref="B2" r:id="rId1" location="" tooltip="" display="a@z3.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>